<commit_message>
add epic subpage and backlog subpage
</commit_message>
<xml_diff>
--- a/Component Specification.xlsx
+++ b/Component Specification.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="1520" yWindow="0" windowWidth="21220" windowHeight="15620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Storyboard- Active Sprint" sheetId="1" r:id="rId1"/>
+    <sheet name="Epic" sheetId="2" r:id="rId2"/>
+    <sheet name="Storyboard- Backlog" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="51">
   <si>
     <t>Field Name</t>
   </si>
@@ -119,17 +121,113 @@
   <si>
     <t xml:space="preserve">Alphanumeric
 Special chars : Spaces </t>
+  </si>
+  <si>
+    <t>EM_E_1</t>
+  </si>
+  <si>
+    <t>Options for sorting Epics on the Epics page</t>
+  </si>
+  <si>
+    <t>Product
+Owner</t>
+  </si>
+  <si>
+    <t>EM_E_2</t>
+  </si>
+  <si>
+    <t>textfield to enter text to filter Epics</t>
+  </si>
+  <si>
+    <t>SB_B_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>textfield to enter text to filter issues</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filterByText</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contain text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Filter issues by selecting a project</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type
+Owner
+Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project names</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SB_B_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SB_B_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type/Owner/Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options on navigation bar for sorting issues on the backlog page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Select in 3 buttons</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -151,8 +249,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -161,8 +267,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="9">
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="7" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -493,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -654,6 +768,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -661,4 +776,318 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="30">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1"/>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="60">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45">
+      <c r="A3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>